<commit_message>
se incluyenron algunos DaTsource en el proyecto: (en esta versión los DataSources se tuvieron que configurar en mi laptop porque el servidor de Ranorex está apagado)
</commit_message>
<xml_diff>
--- a/DataSource/DataSource - Endoso - ABM_Ajuste.xlsx
+++ b/DataSource/DataSource - Endoso - ABM_Ajuste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\DataSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB00943C-CCCD-40F7-B9B9-8CBA92065EFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8FE328-1552-4890-A683-977C09309DBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Usuario</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>NuevoPorcentajeAjuste</t>
+  </si>
+  <si>
+    <t>https://i-preproducciongestion.segurossura.com.ar/pc/PolicyCenter.do</t>
+  </si>
+  <si>
+    <t>i-preproducciongestion.segurossura.com.ar</t>
+  </si>
+  <si>
+    <t>silverarrow</t>
+  </si>
+  <si>
+    <t>04104013020</t>
   </si>
 </sst>
 </file>
@@ -108,10 +120,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -393,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F3" sqref="F3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,9 +467,33 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{F886309B-10CE-4A4F-A29F-9A193462FF04}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{E3526048-5EB1-47F2-AB35-C453FFFD8455}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>